<commit_message>
almost complete with sheet one
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -8,15 +8,102 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milan\Desktop\Appwelt\expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6692BF-DEA7-4029-884A-E82CF26F332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9FDED2-1CD9-44E4-A3BE-A201A446E524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw_data_01" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="27">
+  <si>
+    <t>RAW DATA</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Category Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Payment Mode</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Complaint</t>
+  </si>
+  <si>
+    <t>04-11-2023</t>
+  </si>
+  <si>
+    <t>18:14:15</t>
+  </si>
+  <si>
+    <t>farmer</t>
+  </si>
+  <si>
+    <t>apply for expenses unknown unknown expenses unknown for testing purpose</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>this is the complaint raised by the farmer of the poltry farm of the pune</t>
+  </si>
+  <si>
+    <t>18:14:16</t>
+  </si>
+  <si>
+    <t>18:14:17</t>
+  </si>
+  <si>
+    <t>18:14:18</t>
+  </si>
+  <si>
+    <t>18:14:19</t>
+  </si>
+  <si>
+    <t>18:14:20</t>
+  </si>
+  <si>
+    <t>18:14:21</t>
+  </si>
+  <si>
+    <t>18:14:22</t>
+  </si>
+  <si>
+    <t>18:14:23</t>
+  </si>
+  <si>
+    <t>18:14:24</t>
+  </si>
+  <si>
+    <t>18:14:25</t>
+  </si>
+  <si>
+    <t>18:14:26</t>
+  </si>
+  <si>
+    <t>18:14:27</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50,8 +137,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,10 +435,469 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="39" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>101</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>101</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>101</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>101</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>101</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>101</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>101</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
+        <v>101</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <v>101</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>101</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2">
+        <v>101</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>101</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2">
+        <v>101</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2">
+        <v>101</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2">
+        <v>101</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>45264</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correct text wrap length
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milan\Desktop\Appwelt\expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9FDED2-1CD9-44E4-A3BE-A201A446E524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D630E64F-F6CD-4E74-BC70-4EC6E0AAFC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>RAW DATA</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Category Code</t>
+    <t>id</t>
   </si>
   <si>
     <t>Description</t>
@@ -50,10 +50,10 @@
     <t>Complaint</t>
   </si>
   <si>
-    <t>04-11-2023</t>
-  </si>
-  <si>
-    <t>18:14:15</t>
+    <t>06-11-2023</t>
+  </si>
+  <si>
+    <t>15:36:11</t>
   </si>
   <si>
     <t>farmer</t>
@@ -68,40 +68,22 @@
     <t>this is the complaint raised by the farmer of the poltry farm of the pune</t>
   </si>
   <si>
-    <t>18:14:16</t>
-  </si>
-  <si>
-    <t>18:14:17</t>
-  </si>
-  <si>
-    <t>18:14:18</t>
-  </si>
-  <si>
-    <t>18:14:19</t>
-  </si>
-  <si>
-    <t>18:14:20</t>
-  </si>
-  <si>
-    <t>18:14:21</t>
-  </si>
-  <si>
-    <t>18:14:22</t>
-  </si>
-  <si>
-    <t>18:14:23</t>
-  </si>
-  <si>
-    <t>18:14:24</t>
-  </si>
-  <si>
-    <t>18:14:25</t>
-  </si>
-  <si>
-    <t>18:14:26</t>
-  </si>
-  <si>
-    <t>18:14:27</t>
+    <t>15:36:45</t>
+  </si>
+  <si>
+    <t>15:36:46</t>
+  </si>
+  <si>
+    <t>15:36:47</t>
+  </si>
+  <si>
+    <t>15:36:48</t>
+  </si>
+  <si>
+    <t>15:36:49</t>
+  </si>
+  <si>
+    <t>15:36:50</t>
   </si>
 </sst>
 </file>
@@ -137,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,7 +134,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,20 +426,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="39" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -499,7 +481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -679,219 +661,6 @@
       </c>
       <c r="H9" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2">
-        <v>101</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2">
-        <v>101</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2">
-        <v>101</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2">
-        <v>101</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2">
-        <v>101</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2">
-        <v>101</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2">
-        <v>101</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2">
-        <v>101</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>45264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>